<commit_message>
Student Management - Academic Year Code Implementation
</commit_message>
<xml_diff>
--- a/StudentManagement_API/ApprovedHistoryExport.xlsx
+++ b/StudentManagement_API/ApprovedHistoryExport.xlsx
@@ -44,7 +44,7 @@
     <t>ApprovedBy</t>
   </si>
   <si>
-    <t>John 1 A. Doe</t>
+    <t>John A. Doe</t>
   </si>
   <si>
     <t>ADM001</t>
@@ -56,7 +56,7 @@
     <t>Section A</t>
   </si>
   <si>
-    <t>23-02-2025</t>
+    <t>26-03-2025</t>
   </si>
   <si>
     <t>Father</t>
@@ -65,10 +65,10 @@
     <t>Michael B. Doe</t>
   </si>
   <si>
-    <t>Meera Kapoor was not available</t>
-  </si>
-  <si>
-    <t>Shahid Kapoor</t>
+    <t>Student requires early pickup due to health concerns</t>
+  </si>
+  <si>
+    <t>Meera Kapoor</t>
   </si>
   <si>
     <t>John Smith</t>
@@ -130,8 +130,8 @@
     <col min="5" max="5" width="12.76648998260498" customWidth="1"/>
     <col min="6" max="6" width="12.210966110229492" customWidth="1"/>
     <col min="7" max="7" width="13.922554969787598" customWidth="1"/>
-    <col min="8" max="8" width="28.927854537963867" customWidth="1"/>
-    <col min="9" max="9" width="13.422276496887207" customWidth="1"/>
+    <col min="8" max="8" width="47.102603912353516" customWidth="1"/>
+    <col min="9" max="9" width="13.281092643737793" customWidth="1"/>
     <col min="10" max="10" width="11.437528610229492" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>